<commit_message>
additional data to add program element name when it's not available in the datasource
</commit_message>
<xml_diff>
--- a/inst/extdata/mapping.xlsx
+++ b/inst/extdata/mapping.xlsx
@@ -1,32 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirst\Sync\USAID Moz\budget_IHO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirst\Sync\USAID Moz\blingr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3FD107-7263-4D96-848D-C1958E2E233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777F3824-2DB5-49DF-85C0-7AE51C356AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old program element" sheetId="1" r:id="rId1"/>
     <sheet name="program_area-name" sheetId="2" r:id="rId2"/>
+    <sheet name="program_element_name" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">program_element_name!$A$1:$B$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="198">
   <si>
     <t>A047</t>
   </si>
@@ -173,13 +188,460 @@
   </si>
   <si>
     <t>A&amp;O</t>
+  </si>
+  <si>
+    <t>Program Design and Learning</t>
+  </si>
+  <si>
+    <t>Administration and Oversight</t>
+  </si>
+  <si>
+    <t>Water Supply and Sanitation</t>
+  </si>
+  <si>
+    <t>PO.1.1</t>
+  </si>
+  <si>
+    <t>PO.2.1</t>
+  </si>
+  <si>
+    <t>A097</t>
+  </si>
+  <si>
+    <t>Program Support</t>
+  </si>
+  <si>
+    <t>HL.1.2</t>
+  </si>
+  <si>
+    <t>Tuberculosis</t>
+  </si>
+  <si>
+    <t>Maternal and Child Health</t>
+  </si>
+  <si>
+    <t>Family Planning and Reproductive Health</t>
+  </si>
+  <si>
+    <t>Sexual Prevention - Abstinence/Be Faithful</t>
+  </si>
+  <si>
+    <t>HL.7.1</t>
+  </si>
+  <si>
+    <t>HL.1.5</t>
+  </si>
+  <si>
+    <t>HL.1.8</t>
+  </si>
+  <si>
+    <t>HL.1.9</t>
+  </si>
+  <si>
+    <t>HL.1.10</t>
+  </si>
+  <si>
+    <t>HL.1.11</t>
+  </si>
+  <si>
+    <t>HL.1.13</t>
+  </si>
+  <si>
+    <t>HL.2.1</t>
+  </si>
+  <si>
+    <t>HL.1.14</t>
+  </si>
+  <si>
+    <t>HL.1.15</t>
+  </si>
+  <si>
+    <t>HL.1.16</t>
+  </si>
+  <si>
+    <t>HL.1.17</t>
+  </si>
+  <si>
+    <t>HL.1.18</t>
+  </si>
+  <si>
+    <t>Service Delivery</t>
+  </si>
+  <si>
+    <t>Sexual Prevention - Other Sexual Prevention</t>
+  </si>
+  <si>
+    <t>Orphans and Vulnerable Children</t>
+  </si>
+  <si>
+    <t>Counseling and Testing</t>
+  </si>
+  <si>
+    <t>Treatment/ARV Drugs</t>
+  </si>
+  <si>
+    <t>Treatment/Adult Treatment</t>
+  </si>
+  <si>
+    <t>Health System Strengthening</t>
+  </si>
+  <si>
+    <t>Universal Access to TB Diagnosis and Treatment</t>
+  </si>
+  <si>
+    <t>Strategic Information</t>
+  </si>
+  <si>
+    <t>Biomedical Prevention - Medical Male Circumcision</t>
+  </si>
+  <si>
+    <t>Biomedical Prevention - Prevention Among Drug Users</t>
+  </si>
+  <si>
+    <t>Pediatric Care and Support</t>
+  </si>
+  <si>
+    <t>Treatment/Pediatric Treatment</t>
+  </si>
+  <si>
+    <t>HL.2.2</t>
+  </si>
+  <si>
+    <t>Improved TB Drug Management</t>
+  </si>
+  <si>
+    <t>HL.2.5</t>
+  </si>
+  <si>
+    <t>Treatment and Support Services</t>
+  </si>
+  <si>
+    <t>HL.2.9</t>
+  </si>
+  <si>
+    <t>HL.2.11</t>
+  </si>
+  <si>
+    <t>HL.3.3</t>
+  </si>
+  <si>
+    <t>HL.3.4</t>
+  </si>
+  <si>
+    <t>HL.3.6</t>
+  </si>
+  <si>
+    <t>HL.3.7</t>
+  </si>
+  <si>
+    <t>TB Laboratory Strengthening</t>
+  </si>
+  <si>
+    <t>Improved TB Infection Prevention and Control</t>
+  </si>
+  <si>
+    <t>Indoor Residual Spraying (IRS) to Prevent Malaria</t>
+  </si>
+  <si>
+    <t>Intermittent Preventive Treatment of Pregnant Women</t>
+  </si>
+  <si>
+    <t>Malaria Research</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (Malaria)</t>
+  </si>
+  <si>
+    <t>HL.3.9</t>
+  </si>
+  <si>
+    <t>HL.6.2</t>
+  </si>
+  <si>
+    <t>HL.6.3</t>
+  </si>
+  <si>
+    <t>HL.6.4</t>
+  </si>
+  <si>
+    <t>HL.6.6</t>
+  </si>
+  <si>
+    <t>HL.6.8</t>
+  </si>
+  <si>
+    <t>HL.7.2</t>
+  </si>
+  <si>
+    <t>HL.7.3</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems (Malaria)</t>
+  </si>
+  <si>
+    <t>Treatment of Obstetric Complications and Disabilities</t>
+  </si>
+  <si>
+    <t>Newborn Care and Treatment</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>Treatment of Child Illness</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening</t>
+  </si>
+  <si>
+    <t>Communication and Knowledge Management (FP/RH)</t>
+  </si>
+  <si>
+    <t>Policy Analysis and Capacity Building</t>
+  </si>
+  <si>
+    <t>HL.7.6</t>
+  </si>
+  <si>
+    <t>HL.3.1</t>
+  </si>
+  <si>
+    <t>Procurement and Supply Chain (FP/RH)</t>
+  </si>
+  <si>
+    <t>Diagnosis and Treatment w Artemisinin-Based Combo Therapies</t>
+  </si>
+  <si>
+    <t>HL.6.1</t>
+  </si>
+  <si>
+    <t>Birth Preparedness and Maternity Services</t>
+  </si>
+  <si>
+    <t>HL.4.2</t>
+  </si>
+  <si>
+    <t>HL.4.4</t>
+  </si>
+  <si>
+    <t>Animal and Human Disease Surveillance</t>
+  </si>
+  <si>
+    <t>Behavior Change Communications</t>
+  </si>
+  <si>
+    <t>HL.4.5</t>
+  </si>
+  <si>
+    <t>HL.4.7</t>
+  </si>
+  <si>
+    <t>Response to Disease Outbreak</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems (PIOET)</t>
+  </si>
+  <si>
+    <t>HL.2.4</t>
+  </si>
+  <si>
+    <t>Programmatic Management of Multi Drug-Resistant TB (MDR-TB)</t>
+  </si>
+  <si>
+    <t>HL.2.8</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems</t>
+  </si>
+  <si>
+    <t>HL.3.2</t>
+  </si>
+  <si>
+    <t>Insecticide-Treated Nets (ITNs) to Prevent Malaria</t>
+  </si>
+  <si>
+    <t>HL.4.1</t>
+  </si>
+  <si>
+    <t>Planning and Preparedness for Outbreak Response</t>
+  </si>
+  <si>
+    <t>HL.1.7</t>
+  </si>
+  <si>
+    <t>TB/HIV</t>
+  </si>
+  <si>
+    <t>HL.9.1</t>
+  </si>
+  <si>
+    <t>Promotion of Improved Nutrition Practices</t>
+  </si>
+  <si>
+    <t>HL.9.5</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems (Nutrition)</t>
+  </si>
+  <si>
+    <t>A082</t>
+  </si>
+  <si>
+    <t>Other Public Health Threats</t>
+  </si>
+  <si>
+    <t>Strengthen Microenterprise Productivity</t>
+  </si>
+  <si>
+    <t>HL.1.1</t>
+  </si>
+  <si>
+    <t>HL.1.19</t>
+  </si>
+  <si>
+    <t>HL.1.12</t>
+  </si>
+  <si>
+    <t>HL.1.6</t>
+  </si>
+  <si>
+    <t>HL.2.3</t>
+  </si>
+  <si>
+    <t>HL.7.4</t>
+  </si>
+  <si>
+    <t>HL.7.5</t>
+  </si>
+  <si>
+    <t>HL.9.2</t>
+  </si>
+  <si>
+    <t>HL.9.3</t>
+  </si>
+  <si>
+    <t>HL.9.4</t>
+  </si>
+  <si>
+    <t>HL.6.10</t>
+  </si>
+  <si>
+    <t>HL.3.8</t>
+  </si>
+  <si>
+    <t>HL.8.1</t>
+  </si>
+  <si>
+    <t>HL.8.2</t>
+  </si>
+  <si>
+    <t>HL.8.3</t>
+  </si>
+  <si>
+    <t>HL.8.8</t>
+  </si>
+  <si>
+    <t>Preventing Mother-to-Child Transmission (PMTCT)</t>
+  </si>
+  <si>
+    <t>Administration and Oversight (HIV)</t>
+  </si>
+  <si>
+    <t>Laboratory Infrastructure</t>
+  </si>
+  <si>
+    <t>Adult Care and Support</t>
+  </si>
+  <si>
+    <t>Improved Management of TB/HIV Co-infection</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (FP/RH)</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems (FP/RH)</t>
+  </si>
+  <si>
+    <t>Population-based Nutrition Service Delivery</t>
+  </si>
+  <si>
+    <t>Nutrition Enabling Environment and Capacity</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (Nutrition)</t>
+  </si>
+  <si>
+    <t>Host Country Strategic Information Systems (MCH)</t>
+  </si>
+  <si>
+    <t>Anti-microbial Resistance (Malaria)</t>
+  </si>
+  <si>
+    <t>Safe Water Access</t>
+  </si>
+  <si>
+    <t>Basic Sanitation</t>
+  </si>
+  <si>
+    <t>Water and Sanitation Policy and Governance</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (Water)</t>
+  </si>
+  <si>
+    <t>HL.2.10</t>
+  </si>
+  <si>
+    <t>Improved Diagnosis and Treatment of Pediatric TB</t>
+  </si>
+  <si>
+    <t>HL.2.7</t>
+  </si>
+  <si>
+    <t>HL.6.9</t>
+  </si>
+  <si>
+    <t>HL.8.5</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (TB)</t>
+  </si>
+  <si>
+    <t>Anti-microbial Resistance (MCH)</t>
+  </si>
+  <si>
+    <t>Water Resources Productivity</t>
+  </si>
+  <si>
+    <t>6560080.00</t>
+  </si>
+  <si>
+    <t>6560090.00</t>
+  </si>
+  <si>
+    <t>HL.4.3</t>
+  </si>
+  <si>
+    <t>HL.4.6</t>
+  </si>
+  <si>
+    <t>Commodity Stockpile</t>
+  </si>
+  <si>
+    <t>Cross-cutting Health Systems Strengthening (PIOET)</t>
+  </si>
+  <si>
+    <t>program_element</t>
+  </si>
+  <si>
+    <t>program_element_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,16 +655,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,12 +699,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867A1E2E-0C49-46D9-9B74-F1DD8A84165A}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
@@ -766,4 +1282,692 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389E8117-EC66-4E76-8D7F-EA05FD8B8A52}">
+  <dimension ref="A1:B83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="19.68359375" customWidth="1"/>
+    <col min="2" max="2" width="26.5234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B83" xr:uid="{389E8117-EC66-4E76-8D7F-EA05FD8B8A52}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B83">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>